<commit_message>
update alda 20 mei
</commit_message>
<xml_diff>
--- a/data_binding_alda.xlsx
+++ b/data_binding_alda.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\git\LMSUpdate18Mei\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36B36BB-364F-48D1-92E8-856CDDEAAF9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB18B9B4-F5DC-4DF2-B0C6-6D0065477D5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{4A4A12A6-C228-4AC0-97A6-EBDFD1F6AF5B}"/>
+    <workbookView xWindow="1140" yWindow="0" windowWidth="19350" windowHeight="11070" activeTab="1" xr2:uid="{4A4A12A6-C228-4AC0-97A6-EBDFD1F6AF5B}"/>
   </bookViews>
   <sheets>
     <sheet name="pretest posttest - search" sheetId="1" r:id="rId1"/>
+    <sheet name="manage faq - search" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
   <si>
     <t>var_search</t>
   </si>
@@ -69,6 +70,21 @@
   </si>
   <si>
     <t>not found</t>
+  </si>
+  <si>
+    <t>coba8</t>
+  </si>
+  <si>
+    <t>coba1</t>
+  </si>
+  <si>
+    <t>Tes</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>coba390213</t>
   </si>
 </sst>
 </file>
@@ -119,12 +135,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -442,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4BB5D07-D0EA-4906-8049-299C4B5E55BF}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +473,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -519,7 +534,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -539,6 +554,81 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515FAF9F-9994-45AA-9E01-FB1C2374F6C9}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update data binding 27 mei
</commit_message>
<xml_diff>
--- a/data_binding_alda.xlsx
+++ b/data_binding_alda.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\git\LMSUpdate20Mei\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\git\LMS27Mei\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F5171B-6F87-40D1-97B8-BDB8DD90A5A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F2F3D5-C324-4D14-B3FE-00C007A7DB5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="0" windowWidth="19350" windowHeight="11070" activeTab="1" xr2:uid="{4A4A12A6-C228-4AC0-97A6-EBDFD1F6AF5B}"/>
+    <workbookView xWindow="1140" yWindow="0" windowWidth="19350" windowHeight="11070" firstSheet="2" activeTab="2" xr2:uid="{4A4A12A6-C228-4AC0-97A6-EBDFD1F6AF5B}"/>
   </bookViews>
   <sheets>
     <sheet name="pretest posttest - search" sheetId="1" r:id="rId1"/>
     <sheet name="pretest posttest - next page" sheetId="3" r:id="rId2"/>
-    <sheet name="manage faq - search" sheetId="2" r:id="rId3"/>
+    <sheet name="manage faq - new faq" sheetId="4" r:id="rId3"/>
+    <sheet name="manage faq - search" sheetId="2" r:id="rId4"/>
+    <sheet name="manage faq - delete" sheetId="5" r:id="rId5"/>
+    <sheet name="manage faq - edit" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="50">
   <si>
     <t>var_search</t>
   </si>
@@ -46,9 +49,6 @@
     <t>found</t>
   </si>
   <si>
-    <t>benarsalah</t>
-  </si>
-  <si>
     <t>pretest</t>
   </si>
   <si>
@@ -64,27 +64,12 @@
     <t>NEOP CSO</t>
   </si>
   <si>
-    <t>Hasil survey dapat diisi oleh surveyor melalui aplikasi</t>
-  </si>
-  <si>
     <t>vasdgasdtqweh</t>
   </si>
   <si>
     <t>not found</t>
   </si>
   <si>
-    <t>coba8</t>
-  </si>
-  <si>
-    <t>coba1</t>
-  </si>
-  <si>
-    <t>Tes</t>
-  </si>
-  <si>
-    <t>Online</t>
-  </si>
-  <si>
     <t>coba390213</t>
   </si>
   <si>
@@ -104,16 +89,121 @@
   </si>
   <si>
     <t>fail</t>
+  </si>
+  <si>
+    <t>pilihanganda</t>
+  </si>
+  <si>
+    <t>Coba Pilihan Ganda</t>
+  </si>
+  <si>
+    <t>var_question</t>
+  </si>
+  <si>
+    <t>var_answer</t>
+  </si>
+  <si>
+    <t>var_gambar</t>
+  </si>
+  <si>
+    <t>var_tag</t>
+  </si>
+  <si>
+    <t>expected_image</t>
+  </si>
+  <si>
+    <t>question2</t>
+  </si>
+  <si>
+    <t>answer2</t>
+  </si>
+  <si>
+    <t>C:\Users\asus\git\LMS27Mei\gambar_alda.jpg</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>success</t>
+  </si>
+  <si>
+    <t>optional_gambar</t>
+  </si>
+  <si>
+    <t>optional_tag</t>
+  </si>
+  <si>
+    <t>ya</t>
+  </si>
+  <si>
+    <t>tidak</t>
+  </si>
+  <si>
+    <t>ujian</t>
+  </si>
+  <si>
+    <t>question6</t>
+  </si>
+  <si>
+    <t>answer6</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>C:\Users\asus\git\LMS27Mei\gambar_alda.gif</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>coba3</t>
+  </si>
+  <si>
+    <t>cancel</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>question7</t>
+  </si>
+  <si>
+    <t>question8</t>
+  </si>
+  <si>
+    <t>question9</t>
+  </si>
+  <si>
+    <t>question10</t>
+  </si>
+  <si>
+    <t>answer7</t>
+  </si>
+  <si>
+    <t>answer8</t>
+  </si>
+  <si>
+    <t>answer9</t>
+  </si>
+  <si>
+    <t>answer10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -479,7 +569,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +596,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -514,7 +604,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -522,7 +612,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
@@ -530,7 +620,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
@@ -538,7 +628,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
@@ -546,15 +636,15 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>2</v>
@@ -565,15 +655,15 @@
         <v>2000</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -585,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01BDB6C6-EB01-4D73-B9E3-D69E24CC9199}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,49 +687,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>22</v>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -648,11 +741,213 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A268E2B2-06AB-4329-BCF5-25EBCF7FD68E}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="46" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515FAF9F-9994-45AA-9E01-FB1C2374F6C9}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,7 +966,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -679,7 +974,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -687,7 +982,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -695,29 +990,78 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E228B591-DD90-4A20-A8C4-F5F52023A95C}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82D1116-3EE1-4D83-8A9C-3CEB316FE193}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update alda 28 mei 2020
</commit_message>
<xml_diff>
--- a/data_binding_alda.xlsx
+++ b/data_binding_alda.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\git\LMS27Mei\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F2F3D5-C324-4D14-B3FE-00C007A7DB5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06A9E09-C443-49B8-93D1-72B72B45B7A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="0" windowWidth="19350" windowHeight="11070" firstSheet="2" activeTab="2" xr2:uid="{4A4A12A6-C228-4AC0-97A6-EBDFD1F6AF5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="4" activeTab="4" xr2:uid="{4A4A12A6-C228-4AC0-97A6-EBDFD1F6AF5B}"/>
   </bookViews>
   <sheets>
     <sheet name="pretest posttest - search" sheetId="1" r:id="rId1"/>
-    <sheet name="pretest posttest - next page" sheetId="3" r:id="rId2"/>
-    <sheet name="manage faq - new faq" sheetId="4" r:id="rId3"/>
-    <sheet name="manage faq - search" sheetId="2" r:id="rId4"/>
-    <sheet name="manage faq - delete" sheetId="5" r:id="rId5"/>
-    <sheet name="manage faq - edit" sheetId="6" r:id="rId6"/>
+    <sheet name="pretest posttest - add new ques" sheetId="7" r:id="rId2"/>
+    <sheet name="pretest posttest - next page" sheetId="3" r:id="rId3"/>
+    <sheet name="manage modul - new module" sheetId="8" r:id="rId4"/>
+    <sheet name="manage faq - new faq" sheetId="4" r:id="rId5"/>
+    <sheet name="manage faq - search" sheetId="2" r:id="rId6"/>
+    <sheet name="manage faq - delete" sheetId="5" r:id="rId7"/>
+    <sheet name="manage faq - edit" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="96">
   <si>
     <t>var_search</t>
   </si>
@@ -166,35 +168,173 @@
     <t>delete</t>
   </si>
   <si>
-    <t>question7</t>
-  </si>
-  <si>
-    <t>question8</t>
-  </si>
-  <si>
-    <t>question9</t>
-  </si>
-  <si>
-    <t>question10</t>
-  </si>
-  <si>
-    <t>answer7</t>
-  </si>
-  <si>
-    <t>answer8</t>
-  </si>
-  <si>
-    <t>answer9</t>
-  </si>
-  <si>
-    <t>answer10</t>
+    <t>opsi_edit</t>
+  </si>
+  <si>
+    <t>var_question_new</t>
+  </si>
+  <si>
+    <t>var_answer_new</t>
+  </si>
+  <si>
+    <t>var_gambar_new</t>
+  </si>
+  <si>
+    <t>var_tag_new</t>
+  </si>
+  <si>
+    <t>var_search_after_edit</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>pertanyaan</t>
+  </si>
+  <si>
+    <t>question_only</t>
+  </si>
+  <si>
+    <t>answer_only</t>
+  </si>
+  <si>
+    <t>picture_only</t>
+  </si>
+  <si>
+    <t>C:\Users\asus\git\LMS27Mei\gambar_edit_alda.jpg</t>
+  </si>
+  <si>
+    <t>gambar_edit_alda.jpg</t>
+  </si>
+  <si>
+    <t>pass_image</t>
+  </si>
+  <si>
+    <t>apaaja</t>
+  </si>
+  <si>
+    <t>var_category</t>
+  </si>
+  <si>
+    <t>var_tipe_soal</t>
+  </si>
+  <si>
+    <t>var_job_function</t>
+  </si>
+  <si>
+    <t>var_job_position</t>
+  </si>
+  <si>
+    <t>var_module</t>
+  </si>
+  <si>
+    <t>var_technical_comp</t>
+  </si>
+  <si>
+    <t>var_level_comp</t>
+  </si>
+  <si>
+    <t>var_soal</t>
+  </si>
+  <si>
+    <t>var_jawaban_a</t>
+  </si>
+  <si>
+    <t>var_jawaban_b</t>
+  </si>
+  <si>
+    <t>var_jawaban_c</t>
+  </si>
+  <si>
+    <t>var_jawaban_d</t>
+  </si>
+  <si>
+    <t>var_kunci_jawaban</t>
+  </si>
+  <si>
+    <t>var_module_name</t>
+  </si>
+  <si>
+    <t>var_learning_path</t>
+  </si>
+  <si>
+    <t>var_level</t>
+  </si>
+  <si>
+    <t>var_course_name</t>
+  </si>
+  <si>
+    <t>var_module_category</t>
+  </si>
+  <si>
+    <t>var_module_code</t>
+  </si>
+  <si>
+    <t>var_description</t>
+  </si>
+  <si>
+    <t>var_tags</t>
+  </si>
+  <si>
+    <t>var_prerequisite</t>
+  </si>
+  <si>
+    <t>var_status</t>
+  </si>
+  <si>
+    <t>expected_module_details</t>
+  </si>
+  <si>
+    <t>question5</t>
+  </si>
+  <si>
+    <t>question 5 adalah?</t>
+  </si>
+  <si>
+    <t>jawaban pertanyaan 5</t>
+  </si>
+  <si>
+    <t>answer5</t>
+  </si>
+  <si>
+    <t>question 6 adalah?</t>
+  </si>
+  <si>
+    <t>question11</t>
+  </si>
+  <si>
+    <t>question12</t>
+  </si>
+  <si>
+    <t>question13</t>
+  </si>
+  <si>
+    <t>question14</t>
+  </si>
+  <si>
+    <t>question15</t>
+  </si>
+  <si>
+    <t>answer11</t>
+  </si>
+  <si>
+    <t>answer12</t>
+  </si>
+  <si>
+    <t>answer13</t>
+  </si>
+  <si>
+    <t>answer14</t>
+  </si>
+  <si>
+    <t>answer15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,13 +348,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -244,13 +410,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -258,6 +433,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7C80"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -569,20 +749,20 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -651,18 +831,18 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="3">
         <v>2000</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -672,11 +852,70 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93511CE7-8157-43E1-9C86-99A7D875C1F9}">
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01BDB6C6-EB01-4D73-B9E3-D69E24CC9199}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,13 +926,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -729,9 +968,9 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -740,7 +979,87 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{688EB94B-1F65-4403-8324-7F51C64F76D0}">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A268E2B2-06AB-4329-BCF5-25EBCF7FD68E}">
   <dimension ref="A1:H9"/>
   <sheetViews>
@@ -760,179 +1079,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="A4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F4" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="A5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F5" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H5" t="s">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="A6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F7" t="s">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H7" t="s">
+      <c r="G7" s="3"/>
+      <c r="H7" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="A8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H8" t="s">
+      <c r="G8" s="3"/>
+      <c r="H8" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F9" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -942,12 +1280,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515FAF9F-9994-45AA-9E01-FB1C2374F6C9}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,10 +1295,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -989,18 +1327,18 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1009,12 +1347,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E228B591-DD90-4A20-A8C4-F5F52023A95C}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,18 +1362,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1052,16 +1390,327 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82D1116-3EE1-4D83-8A9C-3CEB316FE193}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="47.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update db 28 mei
</commit_message>
<xml_diff>
--- a/data_binding_alda.xlsx
+++ b/data_binding_alda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\git\LMS27Mei\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06A9E09-C443-49B8-93D1-72B72B45B7A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FA64D6-B420-4F47-BA8D-AE56A2DC24BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="4" activeTab="4" xr2:uid="{4A4A12A6-C228-4AC0-97A6-EBDFD1F6AF5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{4A4A12A6-C228-4AC0-97A6-EBDFD1F6AF5B}"/>
   </bookViews>
   <sheets>
     <sheet name="pretest posttest - search" sheetId="1" r:id="rId1"/>
@@ -96,9 +96,6 @@
     <t>pilihanganda</t>
   </si>
   <si>
-    <t>Coba Pilihan Ganda</t>
-  </si>
-  <si>
     <t>var_question</t>
   </si>
   <si>
@@ -328,6 +325,9 @@
   </si>
   <si>
     <t>answer15</t>
+  </si>
+  <si>
+    <t>Di bawah ini adalah unsur-unsur dalam peta, yaitu .........</t>
   </si>
 </sst>
 </file>
@@ -748,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4BB5D07-D0EA-4906-8049-299C4B5E55BF}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,9 +822,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>2</v>
@@ -863,43 +863,43 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
         <v>57</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>58</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>59</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>60</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>61</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>62</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>63</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>64</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>65</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>66</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>67</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>68</v>
-      </c>
-      <c r="M1" t="s">
-        <v>69</v>
       </c>
       <c r="N1" t="s">
         <v>1</v>
@@ -991,62 +991,62 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -1063,7 +1063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A268E2B2-06AB-4329-BCF5-25EBCF7FD68E}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1080,25 +1080,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>1</v>
@@ -1106,25 +1106,25 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>14</v>
@@ -1132,22 +1132,22 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
@@ -1156,21 +1156,21 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>14</v>
@@ -1178,18 +1178,18 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
@@ -1198,19 +1198,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -1220,12 +1220,12 @@
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
@@ -1234,20 +1234,20 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
@@ -1257,18 +1257,18 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>16</v>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -1312,7 +1312,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1320,7 +1320,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -1371,18 +1371,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1416,25 +1416,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>1</v>
@@ -1442,28 +1442,28 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>14</v>
@@ -1471,49 +1471,49 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -1521,21 +1521,21 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
@@ -1544,23 +1544,23 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3" t="s">
@@ -1569,23 +1569,23 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3" t="s">
@@ -1594,20 +1594,20 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>14</v>
@@ -1615,10 +1615,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1632,20 +1632,20 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>14</v>
@@ -1653,10 +1653,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1670,41 +1670,41 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>

</xml_diff>

<commit_message>
update alda 29 mei 2020
</commit_message>
<xml_diff>
--- a/data_binding_alda.xlsx
+++ b/data_binding_alda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\git\LMS27Mei\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FA64D6-B420-4F47-BA8D-AE56A2DC24BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5710B7A-28E9-47DC-AED3-A5C077A0D78B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{4A4A12A6-C228-4AC0-97A6-EBDFD1F6AF5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{4A4A12A6-C228-4AC0-97A6-EBDFD1F6AF5B}"/>
   </bookViews>
   <sheets>
     <sheet name="pretest posttest - search" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="134">
   <si>
     <t>var_search</t>
   </si>
@@ -328,13 +328,127 @@
   </si>
   <si>
     <t>Di bawah ini adalah unsur-unsur dalam peta, yaitu .........</t>
+  </si>
+  <si>
+    <t>Pre-Test</t>
+  </si>
+  <si>
+    <t>Pilihan Ganda</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>RMA</t>
+  </si>
+  <si>
+    <t>NEOP Sales</t>
+  </si>
+  <si>
+    <t>coba</t>
+  </si>
+  <si>
+    <t>Matahari terbenam ke arah?</t>
+  </si>
+  <si>
+    <t>timur</t>
+  </si>
+  <si>
+    <t>utara</t>
+  </si>
+  <si>
+    <t>selatan</t>
+  </si>
+  <si>
+    <t>barat</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Post-Test</t>
+  </si>
+  <si>
+    <t>Benar / Salah</t>
+  </si>
+  <si>
+    <t>NEOP ARHO</t>
+  </si>
+  <si>
+    <t>COVID 19 adalah kepanjangan dari Corona Virus Disease 2019</t>
+  </si>
+  <si>
+    <t>Benar</t>
+  </si>
+  <si>
+    <t>SALES MANAGER</t>
+  </si>
+  <si>
+    <t>Service Basic Training</t>
+  </si>
+  <si>
+    <t>tesst</t>
+  </si>
+  <si>
+    <t>Salah</t>
+  </si>
+  <si>
+    <t>Uraian</t>
+  </si>
+  <si>
+    <t>SERVICE</t>
+  </si>
+  <si>
+    <t>FINANCE &amp; BANKING OFFICER</t>
+  </si>
+  <si>
+    <t>NEOP Teller Cash &amp; PDC, dan FAB</t>
+  </si>
+  <si>
+    <t>testest</t>
+  </si>
+  <si>
+    <t>Mata uang negara Indonesia adalah?</t>
+  </si>
+  <si>
+    <t>Rupiah</t>
+  </si>
+  <si>
+    <t>UNDERWRITING</t>
+  </si>
+  <si>
+    <t>CREDIT ANALYST</t>
+  </si>
+  <si>
+    <t>NEOP Credit Analyst</t>
+  </si>
+  <si>
+    <t>Matahari terbit dari?</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>1x1?</t>
+  </si>
+  <si>
+    <t>coba soal uraian</t>
+  </si>
+  <si>
+    <t>jawaban uraian</t>
+  </si>
+  <si>
+    <t>huruf pertama abjad adalah z?</t>
+  </si>
+  <si>
+    <t>huruf pertama abjad adalah a?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,6 +466,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -410,7 +530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -427,6 +547,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,7 +869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4BB5D07-D0EA-4906-8049-299C4B5E55BF}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -853,60 +974,701 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93511CE7-8157-43E1-9C86-99A7D875C1F9}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="E21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="19" style="6" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="29.28515625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="6" customWidth="1"/>
+    <col min="11" max="11" width="16" style="6" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="6" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" style="6" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" style="6" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="6"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="6" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" s="6">
+        <v>3</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="6">
+        <v>4</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" s="6">
+        <v>2</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="6">
+        <v>5</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N9" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" s="6">
+        <v>3</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G16" s="6">
+        <v>3</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G17" s="6">
+        <v>3</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G18" s="6">
+        <v>3</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="N23" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>